<commit_message>
Add more tests for invalid ingest manifests
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/bad_offset_manifest.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/bad_offset_manifest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="812" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Depositor Batch Thursday 8/22</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Internet Archive</t>
-  </si>
-  <si>
-    <t>Promotion</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -262,23 +259,23 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8777777777778"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.5037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.5037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.8481481481481"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.8518518518519"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="10.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.5037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.5037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.0148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="10.5037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.8481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8518518518519"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.5037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -288,8 +285,8 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -298,40 +295,40 @@
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="M2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -343,81 +340,69 @@
         <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="0" t="n">
+        <v>1999</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1999</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>2013</v>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>1999</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>2013</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="F4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>